<commit_message>
delete text file in resource
</commit_message>
<xml_diff>
--- a/com.ssidApp/src/main/resources/Book.xlsx
+++ b/com.ssidApp/src/main/resources/Book.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colbi\OneDrive\Desktop\Test_Android\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F51AEB-082B-43E2-AD55-82608C3BA28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4E24BEFC-6683-458B-8EC4-095A789A198C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="812" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,8 @@
     <sheet name="MultiToken" sheetId="4" r:id="rId4"/>
     <sheet name="YIDINDJI" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:J5"/>
 </workbook>
 </file>
 
@@ -1535,6 +1531,30 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1547,28 +1567,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1580,7 +1579,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1593,9 +1592,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1822,9 +1818,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="D2:H23"/>
+  <dimension ref="A2:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -2124,7 +2120,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
@@ -2141,14 +2137,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="49" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="50"/>
+      <c r="D1" s="58"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
@@ -2163,13 +2159,13 @@
       <c r="D2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
@@ -2198,13 +2194,13 @@
       <c r="D4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
@@ -2234,14 +2230,14 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="49" t="s">
+      <c r="B7" s="58"/>
+      <c r="C7" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="50"/>
+      <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
@@ -2292,62 +2288,62 @@
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="57"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="51"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="57"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="51"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="57"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="60">
+      <c r="B17" s="49">
         <v>2.34</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="57"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="22" spans="1:4" ht="15.75" customHeight="1"/>
@@ -3331,18 +3327,18 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B13" r:id="rId1" tooltip="mailto:vivek.sarawgi@squbix.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -3355,9 +3351,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -3372,14 +3368,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="57"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="7" t="s">
@@ -3394,13 +3390,13 @@
       <c r="D2" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="7" t="s">
@@ -3429,13 +3425,13 @@
       <c r="D4" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="9" t="s">
@@ -3465,14 +3461,14 @@
       <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="63" t="s">
+      <c r="B7" s="51"/>
+      <c r="C7" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="57"/>
+      <c r="D7" s="51"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="7" t="s">
@@ -3517,62 +3513,62 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="57"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="57"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="51"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="57"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="51"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="57"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="60">
+      <c r="B17" s="49">
         <v>1.34</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="57"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="22" spans="1:4" ht="15.75" customHeight="1"/>
@@ -4556,18 +4552,18 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -4600,14 +4596,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="57"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1">
       <c r="A2" s="7" t="s">
@@ -4622,13 +4618,13 @@
       <c r="D2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="7" t="s">
@@ -4657,13 +4653,13 @@
       <c r="D4" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="9" t="s">
@@ -4695,14 +4691,14 @@
       <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="63" t="s">
+      <c r="B7" s="51"/>
+      <c r="C7" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="57"/>
+      <c r="D7" s="51"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="7" t="s">
@@ -4754,77 +4750,77 @@
       <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="57"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="57"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="51"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="57"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="51"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1">
       <c r="A15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1">
       <c r="A16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="57"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="60">
+      <c r="B17" s="49">
         <v>2.34</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="57"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="A6" xr:uid="{00000000-0002-0000-0300-000000000000}">
@@ -4858,14 +4854,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="49" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="50"/>
+      <c r="D1" s="58"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
@@ -4880,13 +4876,13 @@
       <c r="D2" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
@@ -4915,13 +4911,13 @@
       <c r="D4" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
@@ -4951,14 +4947,14 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="49" t="s">
+      <c r="B7" s="58"/>
+      <c r="C7" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="50"/>
+      <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
@@ -5009,77 +5005,77 @@
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="69">
+      <c r="B17" s="65">
         <v>1.34</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B13" r:id="rId1" tooltip="mailto:tirix59303@100xbit.com" xr:uid="{00000000-0004-0000-0400-000000000000}"/>

</xml_diff>